<commit_message>
first draft of 03_import.qmd completed; moved content from intro3, intro4, intro5.
</commit_message>
<xml_diff>
--- a/data/candidaemias.xlsx
+++ b/data/candidaemias.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\andre\Docu recenti\LSHTM\Other modules\Intro to R\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://phecloud-my.sharepoint.com/personal/andrea_mazzella_ukhsa_gov_uk/Documents/Documents/IntRo/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC5E02D3-9E1B-4EC8-BE53-B7BDC8DCF0ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{14D5A314-1769-4EA8-A42B-2F548DFA4C65}"/>
+    <workbookView xWindow="-22104" yWindow="936" windowWidth="17280" windowHeight="9024" xr2:uid="{14D5A314-1769-4EA8-A42B-2F548DFA4C65}"/>
   </bookViews>
   <sheets>
     <sheet name="site5" sheetId="1" r:id="rId1"/>
@@ -991,46 +991,6 @@
   <dxfs count="16">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1147,6 +1107,54 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1201,21 +1209,13 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <color rgb="FF9C0006"/>
       </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1354,11 +1354,11 @@
     <sortCondition ref="A1:A17"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{4418CE48-AFF2-44BC-BC35-C1529D6FCB28}" name="id" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{505E0C62-C0BD-4131-A34A-4E9299C924EA}" name="timing_A" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{4418CE48-AFF2-44BC-BC35-C1529D6FCB28}" name="id" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{505E0C62-C0BD-4131-A34A-4E9299C924EA}" name="timing_A" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{BC468704-2F4D-42F5-96DC-4A134186C448}" name="cfu_A"/>
     <tableColumn id="4" xr3:uid="{3ADBEE5A-75C9-4D28-AD1E-1072A9C420E3}" name="pcr_A"/>
-    <tableColumn id="7" xr3:uid="{2CAEB8DC-8F75-409B-9B52-4459DF24D317}" name="timing_B" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{2CAEB8DC-8F75-409B-9B52-4459DF24D317}" name="timing_B" dataDxfId="9"/>
     <tableColumn id="3" xr3:uid="{4CBD3CB7-F0FA-47A5-B6E5-26B6C89FF1AD}" name="cfu_B"/>
     <tableColumn id="5" xr3:uid="{3C715A7C-AD04-4E8B-9FAB-E1D295D7854B}" name="pcr_B"/>
     <tableColumn id="8" xr3:uid="{C6B2030B-E38E-4508-85A5-20E3E3AA466F}" name="timing_C"/>
@@ -1376,7 +1376,7 @@
     <sortCondition ref="A1:A37"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{A180E23C-3E6B-4007-A7A9-8451863B5E71}" name="id" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{A180E23C-3E6B-4007-A7A9-8451863B5E71}" name="id" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{03228A0A-D7E5-41DE-B455-9AE7F0DBB73B}" name="age"/>
     <tableColumn id="3" xr3:uid="{BA9019B4-42E5-4C87-ADEC-8B6307902E22}" name="gender"/>
     <tableColumn id="4" xr3:uid="{5E9BC603-C9B6-4384-B27E-E3982EDBD9E4}" name="ethnicity"/>
@@ -1389,8 +1389,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D5DD4F60-D985-4B4B-BE92-860960190477}" name="Table5" displayName="Table5" ref="A1:D42" totalsRowShown="0">
   <autoFilter ref="A1:D42" xr:uid="{D5DD4F60-D985-4B4B-BE92-860960190477}"/>
   <tableColumns count="4">
-    <tableColumn id="3" xr3:uid="{54F80402-8AF4-44BB-998D-F4A71993A62E}" name="key" dataDxfId="8"/>
-    <tableColumn id="1" xr3:uid="{A1B1617B-BDFE-4C18-A308-7C340941DDC6}" name="id" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{54F80402-8AF4-44BB-998D-F4A71993A62E}" name="key" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{A1B1617B-BDFE-4C18-A308-7C340941DDC6}" name="id" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{E79F0FD7-41F7-4554-A30E-C9CA6A76A93E}" name="antifungal"/>
     <tableColumn id="4" xr3:uid="{5F65A447-9844-46E8-8FF2-B9A44D5DB3CA}" name="days"/>
   </tableColumns>
@@ -1413,13 +1413,13 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{855EF3C5-4A5B-4CCB-9064-D6484314F71E}" name="Table3" displayName="Table3" ref="A1:G26" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{855EF3C5-4A5B-4CCB-9064-D6484314F71E}" name="Table3" displayName="Table3" ref="A1:G26" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A1:G26" xr:uid="{855EF3C5-4A5B-4CCB-9064-D6484314F71E}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{5F4874F4-2B72-42C9-9EE6-31F0AC2B2CEC}" name="column_name" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{5F4874F4-2B72-42C9-9EE6-31F0AC2B2CEC}" name="column_name" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{18F80510-C616-4664-ABE0-836F04F1A520}" name="description"/>
     <tableColumn id="3" xr3:uid="{A7EB40BC-F077-4AB9-B4A6-22F290512067}" name="type"/>
-    <tableColumn id="4" xr3:uid="{CE6AF2D8-23ED-490D-9B30-7902AE045AE5}" name="min" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{CE6AF2D8-23ED-490D-9B30-7902AE045AE5}" name="min" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{EEA40043-365C-4B03-A4E4-6D31D64183ED}" name="max"/>
     <tableColumn id="7" xr3:uid="{7A5AE604-97EC-43CC-A995-BC2E6741363F}" name="unit"/>
     <tableColumn id="6" xr3:uid="{1C7F4C1C-E756-40EE-9F11-10783BC11E99}" name="levels"/>
@@ -1727,18 +1727,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B4EADD2-BE48-4F3E-B927-1729205EEA7A}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.88671875" customWidth="1"/>
-    <col min="4" max="8" width="9.109375" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="4" max="8" width="9.140625" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1767,7 +1765,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>5014</v>
       </c>
@@ -1796,7 +1794,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5063</v>
       </c>
@@ -1822,7 +1820,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5082</v>
       </c>
@@ -1842,7 +1840,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5099</v>
       </c>
@@ -1871,7 +1869,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5117</v>
       </c>
@@ -1916,14 +1914,14 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.88671875" customWidth="1"/>
-    <col min="4" max="8" width="9.109375" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="4" max="8" width="9.140625" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1952,7 +1950,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>7020</v>
       </c>
@@ -1972,7 +1970,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>7028</v>
       </c>
@@ -2001,7 +1999,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>7038</v>
       </c>
@@ -2030,7 +2028,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>7068</v>
       </c>
@@ -2056,7 +2054,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>7096</v>
       </c>
@@ -2092,14 +2090,14 @@
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.88671875" customWidth="1"/>
-    <col min="4" max="8" width="9.109375" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="4" max="8" width="9.140625" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2128,7 +2126,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>8003</v>
       </c>
@@ -2151,7 +2149,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>8028</v>
       </c>
@@ -2180,7 +2178,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>8029</v>
       </c>
@@ -2206,7 +2204,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>8035</v>
       </c>
@@ -2235,7 +2233,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>8044</v>
       </c>
@@ -2252,7 +2250,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>8120</v>
       </c>
@@ -2284,22 +2282,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6830A0A-0C76-471A-B738-5DA30E94A5DA}">
   <dimension ref="A1:K72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="8"/>
-    <col min="2" max="2" width="16.44140625" style="8" customWidth="1"/>
-    <col min="3" max="4" width="8.88671875" style="8"/>
-    <col min="5" max="5" width="17.44140625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="8"/>
-    <col min="8" max="8" width="17.5546875" style="8" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="8"/>
+    <col min="1" max="1" width="8.85546875" style="8"/>
+    <col min="2" max="2" width="16.42578125" style="8" customWidth="1"/>
+    <col min="3" max="4" width="8.85546875" style="8"/>
+    <col min="5" max="5" width="17.42578125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="9.140625"/>
+    <col min="7" max="7" width="8.85546875" style="8"/>
+    <col min="8" max="8" width="17.5703125" style="8" customWidth="1"/>
+    <col min="9" max="11" width="9.140625" customWidth="1"/>
+    <col min="12" max="16384" width="8.85546875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2332,7 +2332,7 @@
       </c>
       <c r="K1" s="8"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>5014</v>
       </c>
@@ -2365,7 +2365,7 @@
       </c>
       <c r="K2" s="8"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>5063</v>
       </c>
@@ -2392,7 +2392,7 @@
       </c>
       <c r="K3" s="8"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>5082</v>
       </c>
@@ -2425,7 +2425,7 @@
       </c>
       <c r="K4" s="8"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>5099</v>
       </c>
@@ -2458,7 +2458,7 @@
       </c>
       <c r="K5" s="8"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>5117</v>
       </c>
@@ -2491,7 +2491,7 @@
       </c>
       <c r="K6" s="8"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>7020</v>
       </c>
@@ -2520,7 +2520,7 @@
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>7028</v>
       </c>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="K8" s="8"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>7038</v>
       </c>
@@ -2586,7 +2586,7 @@
       </c>
       <c r="K9" s="8"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>7068</v>
       </c>
@@ -2619,7 +2619,7 @@
       </c>
       <c r="K10" s="8"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>7096</v>
       </c>
@@ -2648,7 +2648,7 @@
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>8003</v>
       </c>
@@ -2677,7 +2677,7 @@
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>8028</v>
       </c>
@@ -2710,7 +2710,7 @@
       </c>
       <c r="K13" s="8"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>8029</v>
       </c>
@@ -2743,7 +2743,7 @@
       </c>
       <c r="K14" s="8"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>8035</v>
       </c>
@@ -2776,7 +2776,7 @@
       </c>
       <c r="K15" s="8"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>8044</v>
       </c>
@@ -2805,7 +2805,7 @@
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>8120</v>
       </c>
@@ -2834,214 +2834,94 @@
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
     </row>
-    <row r="49" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F49" s="8"/>
-      <c r="I49" s="8"/>
-      <c r="J49" s="8"/>
-      <c r="K49" s="8"/>
-    </row>
-    <row r="50" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F50" s="8"/>
-      <c r="I50" s="8"/>
-      <c r="J50" s="8"/>
-      <c r="K50" s="8"/>
-    </row>
-    <row r="51" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F51" s="8"/>
-      <c r="I51" s="8"/>
-      <c r="J51" s="8"/>
-      <c r="K51" s="8"/>
-    </row>
-    <row r="52" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F52" s="8"/>
-      <c r="I52" s="8"/>
-      <c r="J52" s="8"/>
-      <c r="K52" s="8"/>
-    </row>
-    <row r="53" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F53" s="8"/>
-      <c r="I53" s="8"/>
-      <c r="J53" s="8"/>
-      <c r="K53" s="8"/>
-    </row>
-    <row r="54" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F54" s="8"/>
-      <c r="I54" s="8"/>
-      <c r="J54" s="8"/>
-      <c r="K54" s="8"/>
-    </row>
-    <row r="55" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F55" s="8"/>
-      <c r="I55" s="8"/>
-      <c r="J55" s="8"/>
-      <c r="K55" s="8"/>
-    </row>
-    <row r="56" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F56" s="8"/>
-      <c r="I56" s="8"/>
-      <c r="J56" s="8"/>
-      <c r="K56" s="8"/>
-    </row>
-    <row r="57" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F57" s="8"/>
-      <c r="I57" s="8"/>
-      <c r="J57" s="8"/>
-      <c r="K57" s="8"/>
-    </row>
-    <row r="58" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F58" s="8"/>
-      <c r="I58" s="8"/>
-      <c r="J58" s="8"/>
-      <c r="K58" s="8"/>
-    </row>
-    <row r="59" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F59" s="8"/>
-      <c r="I59" s="8"/>
-      <c r="J59" s="8"/>
-      <c r="K59" s="8"/>
-    </row>
-    <row r="60" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F60" s="8"/>
-      <c r="I60" s="8"/>
-      <c r="J60" s="8"/>
-      <c r="K60" s="8"/>
-    </row>
-    <row r="61" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F61" s="8"/>
-      <c r="I61" s="8"/>
-      <c r="J61" s="8"/>
-      <c r="K61" s="8"/>
-    </row>
-    <row r="62" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F62" s="8"/>
-      <c r="I62" s="8"/>
-      <c r="J62" s="8"/>
-      <c r="K62" s="8"/>
-    </row>
-    <row r="63" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F63" s="8"/>
-      <c r="I63" s="8"/>
-      <c r="J63" s="8"/>
-      <c r="K63" s="8"/>
-    </row>
-    <row r="64" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F64" s="8"/>
-      <c r="I64" s="8"/>
-      <c r="J64" s="8"/>
-      <c r="K64" s="8"/>
-    </row>
-    <row r="65" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F65" s="8"/>
-      <c r="I65" s="8"/>
-      <c r="J65" s="8"/>
-      <c r="K65" s="8"/>
-    </row>
-    <row r="66" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F66" s="8"/>
-      <c r="I66" s="8"/>
-      <c r="J66" s="8"/>
-      <c r="K66" s="8"/>
-    </row>
-    <row r="67" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F67" s="8"/>
-      <c r="I67" s="8"/>
-      <c r="J67" s="8"/>
-      <c r="K67" s="8"/>
-    </row>
-    <row r="68" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F68" s="8"/>
-      <c r="I68" s="8"/>
-      <c r="J68" s="8"/>
-      <c r="K68" s="8"/>
-    </row>
-    <row r="69" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F69" s="8"/>
-      <c r="I69" s="8"/>
-      <c r="J69" s="8"/>
-      <c r="K69" s="8"/>
-    </row>
-    <row r="70" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F70" s="8"/>
-      <c r="I70" s="8"/>
-      <c r="J70" s="8"/>
-      <c r="K70" s="8"/>
-    </row>
-    <row r="71" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F71" s="8"/>
-      <c r="I71" s="8"/>
-      <c r="J71" s="8"/>
-      <c r="K71" s="8"/>
-    </row>
-    <row r="72" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F72" s="8"/>
-      <c r="I72" s="8"/>
-      <c r="J72" s="8"/>
-      <c r="K72" s="8"/>
-    </row>
+    <row r="49" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="A1:A37 A73:A1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -3058,12 +2938,12 @@
       <selection activeCell="F1" sqref="A1:F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="14"/>
+    <col min="1" max="16384" width="8.85546875" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>176</v>
       </c>
@@ -3083,7 +2963,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C2" s="14" t="s">
         <v>179</v>
       </c>
@@ -3097,7 +2977,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>181</v>
       </c>
@@ -3117,7 +2997,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>184</v>
       </c>
@@ -3137,7 +3017,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>187</v>
       </c>
@@ -3157,7 +3037,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>190</v>
       </c>
@@ -3171,7 +3051,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>192</v>
       </c>
@@ -3191,7 +3071,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>195</v>
       </c>
@@ -3211,7 +3091,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>198</v>
       </c>
@@ -3231,7 +3111,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>200</v>
       </c>
@@ -3245,7 +3125,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>202</v>
       </c>
@@ -3259,7 +3139,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>204</v>
       </c>
@@ -3279,7 +3159,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>207</v>
       </c>
@@ -3299,7 +3179,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>210</v>
       </c>
@@ -3319,7 +3199,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>213</v>
       </c>
@@ -3333,7 +3213,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>215</v>
       </c>
@@ -3360,14 +3240,14 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="8.88671875" style="8"/>
+    <col min="1" max="3" width="8.85546875" style="8"/>
     <col min="4" max="4" width="21" style="8" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="8"/>
+    <col min="5" max="16384" width="8.85546875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -3381,7 +3261,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>5014</v>
       </c>
@@ -3395,7 +3275,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>5023</v>
       </c>
@@ -3409,7 +3289,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>5028</v>
       </c>
@@ -3423,7 +3303,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>5042</v>
       </c>
@@ -3437,7 +3317,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>5049</v>
       </c>
@@ -3451,7 +3331,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>5063</v>
       </c>
@@ -3465,7 +3345,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>5082</v>
       </c>
@@ -3479,7 +3359,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>5099</v>
       </c>
@@ -3493,7 +3373,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>5117</v>
       </c>
@@ -3507,7 +3387,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>7020</v>
       </c>
@@ -3521,7 +3401,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>7022</v>
       </c>
@@ -3535,7 +3415,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>7028</v>
       </c>
@@ -3549,7 +3429,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>7038</v>
       </c>
@@ -3563,7 +3443,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>7047</v>
       </c>
@@ -3577,7 +3457,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>7054</v>
       </c>
@@ -3591,7 +3471,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>7065</v>
       </c>
@@ -3605,7 +3485,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>7068</v>
       </c>
@@ -3619,7 +3499,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>7088</v>
       </c>
@@ -3633,7 +3513,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>7093</v>
       </c>
@@ -3647,7 +3527,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>7096</v>
       </c>
@@ -3661,7 +3541,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>8003</v>
       </c>
@@ -3675,7 +3555,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>8015</v>
       </c>
@@ -3689,7 +3569,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>8028</v>
       </c>
@@ -3703,7 +3583,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>8029</v>
       </c>
@@ -3717,7 +3597,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>8035</v>
       </c>
@@ -3731,7 +3611,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>8037</v>
       </c>
@@ -3745,7 +3625,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <v>8044</v>
       </c>
@@ -3759,7 +3639,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>8071</v>
       </c>
@@ -3773,7 +3653,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
         <v>8072</v>
       </c>
@@ -3787,7 +3667,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>8076</v>
       </c>
@@ -3801,7 +3681,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <v>8091</v>
       </c>
@@ -3815,7 +3695,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>8097</v>
       </c>
@@ -3829,7 +3709,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
         <v>8105</v>
       </c>
@@ -3843,7 +3723,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <v>8115</v>
       </c>
@@ -3857,7 +3737,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <v>8117</v>
       </c>
@@ -3871,7 +3751,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <v>8120</v>
       </c>
@@ -3885,211 +3765,211 @@
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38"/>
       <c r="B38"/>
       <c r="C38"/>
       <c r="D38"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39"/>
       <c r="B39"/>
       <c r="C39"/>
       <c r="D39"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40"/>
       <c r="B40"/>
       <c r="C40"/>
       <c r="D40"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41"/>
       <c r="B41"/>
       <c r="C41"/>
       <c r="D41"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42"/>
       <c r="B42"/>
       <c r="C42"/>
       <c r="D42"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43"/>
       <c r="B43"/>
       <c r="C43"/>
       <c r="D43"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44"/>
       <c r="B44"/>
       <c r="C44"/>
       <c r="D44"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45"/>
       <c r="B45"/>
       <c r="C45"/>
       <c r="D45"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46"/>
       <c r="B46"/>
       <c r="C46"/>
       <c r="D46"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47"/>
       <c r="B47"/>
       <c r="C47"/>
       <c r="D47"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48"/>
       <c r="B48"/>
       <c r="C48"/>
       <c r="D48"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49"/>
       <c r="B49"/>
       <c r="C49"/>
       <c r="D49"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50"/>
       <c r="B50"/>
       <c r="C50"/>
       <c r="D50"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51"/>
       <c r="B51"/>
       <c r="C51"/>
       <c r="D51"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52"/>
       <c r="B52"/>
       <c r="C52"/>
       <c r="D52"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53"/>
       <c r="B53"/>
       <c r="C53"/>
       <c r="D53"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54"/>
       <c r="B54"/>
       <c r="C54"/>
       <c r="D54"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55"/>
       <c r="B55"/>
       <c r="C55"/>
       <c r="D55"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56"/>
       <c r="B56"/>
       <c r="C56"/>
       <c r="D56"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57"/>
       <c r="B57"/>
       <c r="C57"/>
       <c r="D57"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58"/>
       <c r="B58"/>
       <c r="C58"/>
       <c r="D58"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59"/>
       <c r="B59"/>
       <c r="C59"/>
       <c r="D59"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60"/>
       <c r="B60"/>
       <c r="C60"/>
       <c r="D60"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61"/>
       <c r="B61"/>
       <c r="C61"/>
       <c r="D61"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62"/>
       <c r="B62"/>
       <c r="C62"/>
       <c r="D62"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63"/>
       <c r="B63"/>
       <c r="C63"/>
       <c r="D63"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64"/>
       <c r="B64"/>
       <c r="C64"/>
       <c r="D64"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65"/>
       <c r="B65"/>
       <c r="C65"/>
       <c r="D65"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66"/>
       <c r="B66"/>
       <c r="C66"/>
       <c r="D66"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67"/>
       <c r="B67"/>
       <c r="C67"/>
       <c r="D67"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68"/>
       <c r="B68"/>
       <c r="C68"/>
       <c r="D68"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69"/>
       <c r="B69"/>
       <c r="C69"/>
       <c r="D69"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70"/>
       <c r="B70"/>
       <c r="C70"/>
       <c r="D70"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71"/>
       <c r="B71"/>
       <c r="C71"/>
       <c r="D71"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72"/>
       <c r="B72"/>
       <c r="C72"/>
@@ -4097,7 +3977,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A37 A73:A1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -4114,16 +3994,17 @@
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.88671875" style="8"/>
-    <col min="3" max="3" width="15.5546875" style="8" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" style="8" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="8"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="8"/>
+    <col min="3" max="3" width="15.5703125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>68</v>
       </c>
@@ -4137,7 +4018,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>69</v>
       </c>
@@ -4151,7 +4032,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>70</v>
       </c>
@@ -4165,7 +4046,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>71</v>
       </c>
@@ -4179,7 +4060,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>72</v>
       </c>
@@ -4193,7 +4074,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>73</v>
       </c>
@@ -4207,7 +4088,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>74</v>
       </c>
@@ -4221,7 +4102,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>75</v>
       </c>
@@ -4235,7 +4116,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>76</v>
       </c>
@@ -4249,7 +4130,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>104</v>
       </c>
@@ -4263,7 +4144,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>77</v>
       </c>
@@ -4277,7 +4158,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>78</v>
       </c>
@@ -4291,7 +4172,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>79</v>
       </c>
@@ -4305,7 +4186,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>80</v>
       </c>
@@ -4319,7 +4200,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>81</v>
       </c>
@@ -4333,7 +4214,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>82</v>
       </c>
@@ -4347,7 +4228,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>105</v>
       </c>
@@ -4361,7 +4242,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>83</v>
       </c>
@@ -4375,7 +4256,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>84</v>
       </c>
@@ -4389,7 +4270,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>85</v>
       </c>
@@ -4403,7 +4284,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>86</v>
       </c>
@@ -4417,7 +4298,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>87</v>
       </c>
@@ -4431,7 +4312,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>88</v>
       </c>
@@ -4445,7 +4326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>106</v>
       </c>
@@ -4459,7 +4340,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>89</v>
       </c>
@@ -4473,7 +4354,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>90</v>
       </c>
@@ -4487,7 +4368,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>91</v>
       </c>
@@ -4501,7 +4382,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>92</v>
       </c>
@@ -4515,7 +4396,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>93</v>
       </c>
@@ -4529,7 +4410,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>94</v>
       </c>
@@ -4543,7 +4424,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>107</v>
       </c>
@@ -4557,7 +4438,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>95</v>
       </c>
@@ -4571,7 +4452,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>96</v>
       </c>
@@ -4585,7 +4466,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>97</v>
       </c>
@@ -4599,7 +4480,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>98</v>
       </c>
@@ -4613,7 +4494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>108</v>
       </c>
@@ -4627,7 +4508,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>99</v>
       </c>
@@ -4641,7 +4522,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>100</v>
       </c>
@@ -4655,7 +4536,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>101</v>
       </c>
@@ -4669,7 +4550,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>102</v>
       </c>
@@ -4683,7 +4564,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>103</v>
       </c>
@@ -4697,7 +4578,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
         <v>109</v>
       </c>
@@ -4716,10 +4597,10 @@
     <sortCondition ref="B2:B26"/>
   </sortState>
   <conditionalFormatting sqref="B1:B42 B43:C1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43:C43">
-    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -4736,14 +4617,14 @@
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="8"/>
-    <col min="2" max="2" width="10.77734375" style="8" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="8"/>
+    <col min="1" max="1" width="8.85546875" style="8"/>
+    <col min="2" max="2" width="10.7109375" style="8" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -4751,7 +4632,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>5028</v>
       </c>
@@ -4759,7 +4640,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>5042</v>
       </c>
@@ -4767,7 +4648,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>5063</v>
       </c>
@@ -4775,7 +4656,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>7020</v>
       </c>
@@ -4783,7 +4664,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>7088</v>
       </c>
@@ -4791,7 +4672,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>7096</v>
       </c>
@@ -4799,7 +4680,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>8003</v>
       </c>
@@ -4807,7 +4688,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>8015</v>
       </c>
@@ -4815,7 +4696,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>8028</v>
       </c>
@@ -4823,7 +4704,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>8029</v>
       </c>
@@ -4831,7 +4712,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>8044</v>
       </c>
@@ -4839,7 +4720,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>8076</v>
       </c>
@@ -4847,7 +4728,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>8091</v>
       </c>
@@ -4855,7 +4736,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>8120</v>
       </c>
@@ -4879,17 +4760,17 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.21875" customWidth="1"/>
-    <col min="2" max="2" width="44.5546875" customWidth="1"/>
-    <col min="3" max="3" width="11.77734375" customWidth="1"/>
-    <col min="6" max="6" width="24.21875" customWidth="1"/>
-    <col min="7" max="7" width="83.77734375" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="44.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" customWidth="1"/>
+    <col min="7" max="7" width="83.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>111</v>
       </c>
@@ -4912,7 +4793,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -4929,7 +4810,7 @@
         <v>8999</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -4944,7 +4825,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -4964,7 +4845,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
@@ -4984,7 +4865,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
@@ -5004,7 +4885,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -5024,7 +4905,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>4</v>
       </c>
@@ -5044,7 +4925,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>6</v>
       </c>
@@ -5064,7 +4945,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
@@ -5084,7 +4965,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>113</v>
       </c>
@@ -5104,7 +4985,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>115</v>
       </c>
@@ -5124,7 +5005,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>117</v>
       </c>
@@ -5138,7 +5019,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>114</v>
       </c>
@@ -5158,7 +5039,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>116</v>
       </c>
@@ -5178,7 +5059,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>118</v>
       </c>
@@ -5192,7 +5073,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>127</v>
       </c>
@@ -5212,7 +5093,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>128</v>
       </c>
@@ -5232,7 +5113,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>129</v>
       </c>
@@ -5246,7 +5127,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>46</v>
       </c>
@@ -5266,7 +5147,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>47</v>
       </c>
@@ -5280,7 +5161,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>48</v>
       </c>
@@ -5294,7 +5175,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>68</v>
       </c>
@@ -5306,7 +5187,7 @@
       </c>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>43</v>
       </c>
@@ -5321,7 +5202,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>42</v>
       </c>
@@ -5341,7 +5222,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>37</v>
       </c>

</xml_diff>